<commit_message>
added all photos to wines
</commit_message>
<xml_diff>
--- a/Wine_list.xlsx
+++ b/Wine_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="131">
   <si>
     <t>Name</t>
   </si>
@@ -202,7 +202,10 @@
     <t>Delightful aromas of juicy red cherries, strawberries, rose petals and wild scrub with hints of juniper and chopped herbs. Medium body with firm tannins and lively acidity. Aromatic, spicy and balanced with a nice finish. Fruity finish. Give it time. Try it after 2027.”</t>
   </si>
   <si>
-    <t>Ciacci Brunello di Montacino</t>
+    <t>wines/image13.png</t>
+  </si>
+  <si>
+    <t>Ciacci Brunello di Montalcino</t>
   </si>
   <si>
     <t>Sangiovese</t>
@@ -217,6 +220,9 @@
     <t>Wine and only wine: this champagne dominated by Pinot Noir is made without expedition liqueur. Straw-yellow in color with bright reflections, subtle nose of peaches and apricots with a vegetal touch. In the mouth, honest and unctuous attack, a beautiful harmony and a fine finish. A champagne for connoisseurs!"</t>
   </si>
   <si>
+    <t>wines/image14.png</t>
+  </si>
+  <si>
     <t>Jacques Defrance Brut Tradition</t>
   </si>
   <si>
@@ -229,6 +235,9 @@
     <t>James Suckling: "A hint of flint and gunpowder, with waxy lemon, oyster shell, mango and green apple. A textured and saline expression of Chardonnay with fresh flavors and a mineral tinge. Full-bodied and reductive, with phenolic support. Finish savory, salty and savory. I like the austerity of wine. Drink it or keep it.”</t>
   </si>
   <si>
+    <t>wines/image15.png</t>
+  </si>
+  <si>
     <t>El Enemigo Chardonnay</t>
   </si>
   <si>
@@ -238,6 +247,9 @@
     <t>James Suckling: "Exotic but serious nose of tropical fruits (green mango, papaya), salty lemon, minerals and a touch of whipped cream. On the palate, it's ample, with fresh yet supple acidity and a spicy finish, full of almonds and a hint of bitter aromatic herbs. Deliciously phenolic and structured. Drink it or keep it.”</t>
   </si>
   <si>
+    <t>wines/image16.png</t>
+  </si>
+  <si>
     <t>El Enemigo Semillon 2021</t>
   </si>
   <si>
@@ -247,7 +259,10 @@
     <t>The emblematic variety of Sicily reveals itself in a remarkably fruity, soft and velvety expression. Matured for 6 months in barrels, the wine has intense aromas of raisins, wild strawberries and pomegranate. In the mouth it is velvety, with a beautiful structure and intense fruit aromas. Discover the typicality of the Nero d'Avola variety at a superb quality-price-pleasure ratio!</t>
   </si>
   <si>
-    <t>Feud Arancio Nero d'Avola</t>
+    <t>wines/image17.png</t>
+  </si>
+  <si>
+    <t>Feudo Arancio Nero d'Avola</t>
   </si>
   <si>
     <t>Nero d'Avola</t>
@@ -259,6 +274,9 @@
     <t>Enchanting bouquet of dark red fruits, especially raspberries, blackberries and cherries, with hints of violets and spicy Syrah notes. Elegant, velvety and full-bodied taste, very good structure, refined, delicate and well-integrated tannins and a long, very pleasant finish.</t>
   </si>
   <si>
+    <t>wines/image18.png</t>
+  </si>
+  <si>
     <t>Feud Arancio Nero d'Avola Passiari</t>
   </si>
   <si>
@@ -268,6 +286,9 @@
     <t>Ideal for summer! Beautiful and fruity bouquet of pears, apricots, white and yellow peaches. Elegant, velvety, fragrant and fruity taste, with discreet notes of vanilla.</t>
   </si>
   <si>
+    <t>wines/image19.png</t>
+  </si>
+  <si>
     <t>Feud Arancio Nero d'Avola Inzolia</t>
   </si>
   <si>
@@ -277,6 +298,9 @@
     <t>Warm and tempting, with spicy notes of black pepper and thyme, on a background of cherries and wild fruits. In the mouth it is very pleasant, with velvety tannins.</t>
   </si>
   <si>
+    <t>wines/image20.png</t>
+  </si>
+  <si>
     <t>Feud Arancio Nero d'Avola Syrah</t>
   </si>
   <si>
@@ -286,7 +310,10 @@
     <t>In autumn, the picturesque vineyards of Valdobbiadene are charged with a splendid scent of ripe fruit, a sign that it is time to pick grapes. This is also the moment when Foss Marai extracts the purest essence of the intensely aromatic Glera grapes and builds around them the identity of a wine that surprises the tasting with fabulous aromas, although it maintains a defining traditional line for Strada di Guia 109 Prosecco Valdobbiadene DOCG Extra Dry. The Foss Marai style is generally noted for the excellence with which it manages to reflect the Venetian terroir in the aromatic palettes of its wines, so that this time too we have a particularly interesting aromatic journey, which bears the signature of an area with a tradition in the production of prosecco. A temperature of 8-10 degrees Celsius proves to be ideal to highlight the aperitif qualities of this prosecco, as well as those of a culinary accompaniment to light fish dishes</t>
   </si>
   <si>
-    <t>Ferghettina Franciacorta Milled</t>
+    <t>wines/image21.png</t>
+  </si>
+  <si>
+    <t>Ferghettina Franciacorta Milledi</t>
   </si>
   <si>
     <t>Sparkling White</t>
@@ -295,6 +322,9 @@
     <t>A fantastic quality Franciacorta with an extraordinary minerality! Fine, persistent bubbles introduce a very fresh and elegant bouquet with intense notes of citrus and white flowers. On the palate, the wine is complex and vivacious, with fine, persistent perlage, fresh citrus aromas intertwined with mineral and brioche notes that give it weight and a very fine texture. Strong minerality and tantalizing acidity lead to a lingering, memorable finish.</t>
   </si>
   <si>
+    <t>wines/image22.png</t>
+  </si>
+  <si>
     <t>Gut Hermannsberg 7 Terroirs</t>
   </si>
   <si>
@@ -310,12 +340,18 @@
     <t>7 Terroris is the emblematic cuvee of the house with grapes from the highest areas of all 7 Grosse Lagen parcels, based on the youngest vineyards on the Krupfergrube plain. Starting with the 2020 harvest, this cuvee redefines the Gutwein category. Spontaneous fermentation, mostly in stainless steel but also with some large neutral wood, it has a mineral-smoky-spicy character, it is expressive, energetic and with a distinct, delicate note of grapefruit specific to Krupfergrube.</t>
   </si>
   <si>
+    <t>wines/image23.png</t>
+  </si>
+  <si>
     <t>Gut Hermannsberg Rotenberg Kabinett</t>
   </si>
   <si>
     <t>The classic Kabinett with 9% alcohol and comforting acidity</t>
   </si>
   <si>
+    <t>wines/image24.png</t>
+  </si>
+  <si>
     <t>La Rioja Alta Viña Alberdi Reserva</t>
   </si>
   <si>
@@ -328,12 +364,18 @@
     <t>James Suckling: "Attractive aromas of sweet spices, smoke and seaweed. A little toasted walnut. Hints of Iberian ham. Medium body, nicely rounded tannins and juicy fruit. Pure Tempranillo. Drink it now.”</t>
   </si>
   <si>
-    <t>In Rioja Alta Finca San Martín Crianza</t>
+    <t>wines/image25.png</t>
+  </si>
+  <si>
+    <t>La Rioja Alta Finca San Martín Crianza</t>
   </si>
   <si>
     <t>James Suckling: "A simple and beautiful Rioja with subtle notes of spice, berries, red plums and a bit of orange. On the palate it has medium body, medium acidity, it is round with soft tannins and a creamy finish with medium length. Very approachable. Drink it now.”</t>
   </si>
   <si>
+    <t>wines/image26.png</t>
+  </si>
+  <si>
     <t>Flor de Muga Blanco</t>
   </si>
   <si>
@@ -343,16 +385,10 @@
     <t>Strong aromas with a smoky, creamy undertone. Minerals, toasted white almonds and green stone fruits. Full-bodied and lively, it is aromatic and pure in the middle of the evolution on the palate. A nice touch of phenols and salinity on the finish gives it a bit more gravitas. 40% Viura, 30% Maturana blanca and 30% Garnacha blanca. Drink it or keep it.”</t>
   </si>
   <si>
-    <t>Muga Reserve</t>
-  </si>
-  <si>
-    <t>Temprallino, Granacha Tinta</t>
-  </si>
-  <si>
-    <t>Reserva 2019, sold under the name Criaza" in Spain, comes from a dry and hot year, with low yield and concentrated wines. Tempranillo, Garnacha Tinta, Mazuelo and Graciano grapes fermented destemmed and lightly crushed in oak vats with indigenous yeasts, and 80% of the wine was aged for 22 months in French oak and the rest in Central European and American oak. 20% new barrels. A serious and young wine, but balanced, nuanced and complex. Muga shortens the time spent in the barrel because they have better and younger barrels and have concluded that the wines need less time in oak and more time in the bottle. A very Muga, very Rioja and very good wine. They produced an impressive number of bottles: 960,000, plus 18,000 magnums. A single assemblage bottled on different dates."</t>
-  </si>
-  <si>
-    <t>Muga Rosé</t>
+    <t>wines/image27.png</t>
+  </si>
+  <si>
+    <t>Muga Rosado</t>
   </si>
   <si>
     <t>Granaca Tinta and Viura</t>
@@ -361,10 +397,16 @@
     <t>A beautiful color, pale Provençal pink. Delightful nose of flowers, especially rose petals and almonds. The fruit aromas are also very good - red berries, wild strawberries and some hints of creamy vanilla. On the palate, velvety attack, quite juicy followed by a pleasant acidity that balances the sweet first impression. Then the wine evolves nicely towards the refreshing, aromatic finish. A beautifully balanced rosé of surprising complexity.</t>
   </si>
   <si>
+    <t>wines/image28.png</t>
+  </si>
+  <si>
     <t>Flor de Muga Rosado</t>
   </si>
   <si>
     <t>James Suckling: "Fine chalk, white strawberries and hints of cherry blossoms, whipped cream and minerals. Lively and elegant, it is very dry on the palate and has a savory finish. A serious and gourmet Rosado made from 100% Garnacha. Drink it or keep it.”</t>
+  </si>
+  <si>
+    <t>wines/image29.png</t>
   </si>
 </sst>
 </file>
@@ -382,7 +424,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -414,19 +456,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -449,8 +488,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I31" displayName="Table3" name="Table3" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:I31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I30" displayName="Table3" name="Table3" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:I30"/>
   <tableColumns count="9">
     <tableColumn name="Name" id="1"/>
     <tableColumn name="Type" id="2"/>
@@ -754,25 +793,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="46.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="44.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="46.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="44.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="4" width="17.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -804,14 +843,14 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>2022</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -821,10 +860,10 @@
         <v>13</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="4">
+      <c r="G2" s="2">
         <v>75</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="2">
         <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -834,14 +873,14 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>2023</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -853,10 +892,10 @@
       <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="2">
         <v>110</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="2">
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -866,14 +905,14 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>2020</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -885,10 +924,10 @@
       <c r="F4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="2">
         <v>200</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="2">
         <v>15</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -898,14 +937,14 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>2016</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -915,10 +954,10 @@
         <v>19</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="4">
+      <c r="G5" s="2">
         <v>100</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="2">
         <v>12</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -928,14 +967,14 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>2023</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -945,10 +984,10 @@
         <v>19</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="4">
+      <c r="G6" s="2">
         <v>55</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="2">
         <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -958,14 +997,14 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>2023</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -977,10 +1016,10 @@
       <c r="F7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="2">
         <v>60</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="2">
         <v>20</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -990,14 +1029,14 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <v>2019</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1009,10 +1048,10 @@
       <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="2">
         <v>230</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="2">
         <v>15</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -1022,14 +1061,14 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="2">
         <v>2018</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1041,10 +1080,10 @@
       <c r="F9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="2">
         <v>285</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="2">
         <v>30</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -1054,14 +1093,14 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="2">
         <v>2020</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1073,10 +1112,10 @@
       <c r="F10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="2">
         <v>105</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="2">
         <v>20</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -1086,14 +1125,14 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="2">
         <v>2019</v>
       </c>
       <c r="D11" s="1"/>
@@ -1103,10 +1142,10 @@
       <c r="F11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="2">
         <v>115</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="2">
         <v>10</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -1116,14 +1155,14 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="2">
         <v>2020</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1135,10 +1174,10 @@
       <c r="F12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="2">
         <v>145</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="2">
         <v>12</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -1148,14 +1187,14 @@
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="2">
         <v>2020</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1167,10 +1206,10 @@
       <c r="F13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="2">
         <v>235</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="2">
         <v>40</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -1180,14 +1219,14 @@
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="2">
         <v>2018</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1199,516 +1238,520 @@
       <c r="F14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="2">
         <v>95</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="2">
         <v>12</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J14" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="J14" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="2">
         <v>2019</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G15" s="4">
+        <v>66</v>
+      </c>
+      <c r="G15" s="2">
         <v>280</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="2">
         <v>40</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J15" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+        <v>67</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="4">
+      <c r="G16" s="2">
         <v>180</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="2">
         <v>24</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J16" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+        <v>72</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="2">
         <v>2021</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="4">
+      <c r="G17" s="2">
         <v>105</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="2">
         <v>21</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J17" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+        <v>76</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="2">
         <v>2021</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="4">
+      <c r="G18" s="2">
         <v>106</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="2">
         <v>6</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J18" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+        <v>80</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="2">
         <v>2021</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" s="4">
+        <v>84</v>
+      </c>
+      <c r="G19" s="2">
         <v>40</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="2">
         <v>12</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J19" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+        <v>85</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="2">
         <v>2020</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="4">
+        <v>84</v>
+      </c>
+      <c r="G20" s="2">
         <v>45</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="2">
         <v>18</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J20" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+        <v>89</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="4">
-        <v>2020</v>
+      <c r="C21" s="2">
+        <v>2022</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" s="4">
+        <v>84</v>
+      </c>
+      <c r="G21" s="2">
         <v>40</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="2">
         <v>24</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J21" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+        <v>93</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="2">
         <v>2021</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G22" s="4">
+        <v>84</v>
+      </c>
+      <c r="G22" s="2">
         <v>40</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="2">
         <v>24</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J22" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+        <v>97</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="4">
+        <v>100</v>
+      </c>
+      <c r="C23" s="2">
         <v>2020</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="4">
+      <c r="G23" s="2">
         <v>165</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="2">
         <v>16</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J23" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+        <v>101</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="2">
         <v>2023</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G24" s="4">
+        <v>106</v>
+      </c>
+      <c r="G24" s="2">
         <v>100</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="2">
         <v>8</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="J24" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+        <v>107</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="2">
         <v>2023</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G25" s="4">
+        <v>106</v>
+      </c>
+      <c r="G25" s="2">
         <v>135</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="2">
         <v>8</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J25" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+        <v>110</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="2">
         <v>2019</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G26" s="4">
+        <v>114</v>
+      </c>
+      <c r="G26" s="2">
         <v>110</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="2">
         <v>12</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J26" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+        <v>115</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="4">
-        <v>2021</v>
+      <c r="C27" s="2">
+        <v>2020</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G27" s="4">
+        <v>114</v>
+      </c>
+      <c r="G27" s="2">
         <v>60</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="2">
         <v>12</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J27" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+        <v>118</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="4">
-        <v>2019</v>
+      <c r="C28" s="2">
+        <v>2020</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G28" s="4">
+        <v>114</v>
+      </c>
+      <c r="G28" s="2">
         <v>180</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="2">
         <v>12</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="J28" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+        <v>122</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="4">
-        <v>2021</v>
+      <c r="C29" s="2">
+        <v>2023</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G29" s="4">
-        <v>125</v>
-      </c>
-      <c r="H29" s="4">
+        <v>114</v>
+      </c>
+      <c r="G29" s="2">
+        <v>60</v>
+      </c>
+      <c r="H29" s="2">
         <v>12</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="J29" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+        <v>126</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="2">
         <v>2023</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G30" s="4">
-        <v>60</v>
-      </c>
-      <c r="H30" s="4">
+        <v>114</v>
+      </c>
+      <c r="G30" s="2">
+        <v>120</v>
+      </c>
+      <c r="H30" s="2">
         <v>12</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J30" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="4">
-        <v>2023</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G31" s="4">
-        <v>120</v>
-      </c>
-      <c r="H31" s="4">
-        <v>12</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="J31" s="1"/>
+        <v>129</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>